<commit_message>
Added 2 excel changes
</commit_message>
<xml_diff>
--- a/assets/files/downloads/fm/Financial-Management-Business-Capabilities.xlsx
+++ b/assets/files/downloads/fm/Financial-Management-Business-Capabilities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\courtneyhanderson\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.munipalle\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DC8B426-00DE-4597-8314-47F3CF3EDF5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF73E6DD-5B66-4C87-B7DE-0A19C4FE01B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2290" yWindow="510" windowWidth="14400" windowHeight="7360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,9 +331,6 @@
     <t>Provide budgetary resource reporting attributes (for example, Treasury Account Fund Symbol, expired, and unexpired) consistent with the budget execution activities as defined in OMB Circular No. A-11.</t>
   </si>
   <si>
-    <t>OMB Circular No. A-11, Part 4, Instructions on Budget Execution; OMB Circular No. A-11, Appendix F, Format of SF 132, SF 133, Schedule P, and SBR; OMB Circular No. A-11, Part 4, Section 130, SF 133, Report on Budget Execution and Budgetary Resources; SFFAS 7: Accounting for Revenue and Other Financing Sources and Concepts for Reconciling Budgetary and Financial Accounting</t>
-  </si>
-  <si>
     <t>FFMSR.2.1.1.2</t>
   </si>
   <si>
@@ -382,12 +379,6 @@
     <t>FFM.010.030 Budgetary Reporting</t>
   </si>
   <si>
-    <t>Provide budgetary resource and budget execution data as specified in the TFM to support the budget reporting activities defined in OMB Circular No. A-11, OMB Circular No. A-136, and the FASAB Handbook.</t>
-  </si>
-  <si>
-    <t>OMB Circular No. A-11, Part 4, Instructions on Budget Execution; OMB Circular No. A-11, Part 4, Instructions on Budget Execution, Section 120.29 – Who is responsible for preparing the apportionment request for allocation (parent/child) accounts?; OMB Circular No. A-11, Appendix F, Format of SF 132, SF 133, Schedule P, and SBR; OMB Circular No. A-136, Financial Reporting Requirements, Number II.4.6, Statement of Budgetary Resources; TFM Volume I, Part 2, Chapter 4200 Agency Year-end Reporting on Unexpended Balances of Appropriation Accounts; SFFAS 7: Accounting for Revenue and Other Financing Sources and Concepts for Reconciling Budgetary and Financial Accounting; TFM Volume I, Part 6, Chapter 2100 Fiscal Service Data Registry Additional Reference(s) FFMSR 2.3.2 Verifying Traceability</t>
-  </si>
-  <si>
     <t>FFMSR.2.2.1.1</t>
   </si>
   <si>
@@ -409,21 +400,12 @@
     <t>Capture federal government unique payment information (for example, appropriation and fund) to support payment reports consistent with the TFM.</t>
   </si>
   <si>
-    <t>TFM Volume I, Part 2, Chapter 3100 Instructions for Disbursing Officers' Reports; TFM Volume I, Part 6, Chapter 2100 Fiscal Service Data Registry</t>
-  </si>
-  <si>
     <t>FFMSR.2.2.1.3</t>
   </si>
   <si>
     <t>FFM.030.020 Obligation Management</t>
   </si>
   <si>
-    <t>Determine proper payable amount and other payable information consistent with FASAB Handbook and as specified in the TFM.</t>
-  </si>
-  <si>
-    <t>TFM Volume I, Part 4A, Chapter 3000 Requirements for Scheduling Payments Disbursed by the Bureau of the Fiscal Service; TFM Volume I, Part 4A, Chapter 2000 Overall Disbursing Rules for All Federal Agencies, Section 2070 Preaudit of Vouchers; SFFAS 1: Accounting for Selected Assets and Liabilities; SFFAS 2: Accounting for Direct Loans and Loan Guarantees; SFFAS 5: Accounting for Liabilities of the Federal Government; SFFAS 12: Recognition of Contingent Liabilities Arising from Litigation: An Amendment of SFFAS 5, Accounting for Liabilities of the Federal Government; SFFAS 17: Accounting for Social Insurance; SFFAS 18: Amendments to Accounting Standards for Direct Loans and Loan Guarantees in SFFAS 2; SFFAS 19: Technical Amendments to Accounting Standards for Direct Loans and Loan Guarantees in SFFAS 2</t>
-  </si>
-  <si>
     <t>FFMSR.2.2.1.4</t>
   </si>
   <si>
@@ -749,6 +731,24 @@
   </si>
   <si>
     <t>SFFAS 1: Accounting for Selected Assets and Liabilities; SFFAS 2: Accounting for Direct Loans and Loan Guarantees; SFFAS 5: Accounting for Liabilities of the Federal Government; SFFAS 6: Accounting for Property, Plant, and Equipment; SFFAS 7: Accounting for Revenue and Other Financing Sources and Concepts for Reconciling Budgetary and Financial Accounting; SFFAS 12: Recognition of Contingent Liabilities Arising from Litigation: An Amendment of SFFAS 5, Accounting for Liabilities of the Federal Government; SFFAS 17: Accounting for Social Insurance; SFFAS 18: Amendments to Accounting Standards for Direct Loans and Loan Guarantees in SFFAS 2; SFFAS 19: Technical Amendments to Accounting Standards for Direct Loans and Loan Guarantees in SFFAS 2; SFFAS 33: Pensions, Other Retirement Benefits, and Other Postemployment Benefits: Reporting Gains and Losses from Changes in Assumptions, and Selecting Discount Rates and Valuations Dates  Additional Reference(s) FFMSR 1.1.5 Managing Revenues and Other Financing Sources; FFMSR 1.2.1 Determining Costs    SFFAS 54- Leases: An Amendment of SFFAS 5, Accounting for Liabilities of the Federal Government, and SFFAS 6, Accounting for Property, Plant, and Equipment (Effective for reporting periods beginning after September 30, 2023. Early adoption is not permitted)</t>
+  </si>
+  <si>
+    <t>OMB Circular No. A-11, Preparation, Submission and Execution of the Budget, Part 4, Instructions on Budget Execution;OMB Circular No. A-11, Preparation, Submission and Execution of the Budget, Part 4, Instructions on Budget Execution, Section 130, SF 133, Report on Budget Execution and Budgetary Resources;OMB Circular No. A-11, Preparation, Submission and Execution of the Budget, Appendix F, Format of SF 132, SF 133, Schedule P, and SBR;OMB Circular No. A-11, Preparation, Submission and Execution of the Budget, Appendix H, Checklist for Fund Control Regulations, Section 4: Definitions, Terminology, and Concepts;SFFAS 7: Accounting for Revenue and Other Financing Sources and Concepts for Reconciling Budgetary and Financial Accounting.</t>
+  </si>
+  <si>
+    <t>Provide budgetary resource and budget execution data as specified in the TFM to support the budget reporting activities defined in OMB Circular No. A-11, OMB Circular No. A-136, and the FASAB Handbook</t>
+  </si>
+  <si>
+    <t>OMB Circular No. A-11, Preparation, Submission and Execution of the Budget, Part 4, Instructions on Budget Execution;OMB Circular No. A-11, Preparation, Submission and Execution of the Budget, Part 4, Instructions on Budget Execution, Section 120.29;OMB Circular No. A-11, Preparation, Submission and Execution of the Budget, Appendix F, Format of SF 132, SF 133, Schedule P, and SBR;OMB Circular No. A-136, Financial Reporting Requirements, Number II.3.5, Statement of Budgetary Resources;TFM Volume I, Part 2, Chapter 4200 Agency Year-end Reporting on Unexpended Balances of Appropriation Accounts;TFM Volume I, Part 6, Chapter 2100 Fiscal Service Data Registry;SFFAS 7: Accounting for Revenue and Other Financing Sources and Concepts for Reconciling Budgetary and Financial Accounting;SFFAS 53: Budget and Accrual Reconciliation.</t>
+  </si>
+  <si>
+    <t>TFM Volume I, Part 4A, Chapter 2000 Overall Disbursing Rules for All Federal Agencies;TFM Volume I, Part 6, Chapter 2100 Fiscal Service Data Registry;OMB Circular No. A-11, Preparation, Submission and Execution of the Budget, Part 1, General Information, Section 20: Terms and Concepts;OMB Circular No. A-11, Preparation, Submission and Execution of the Budget, Part 4, Instructions on Budget Execution, Section 120.65;48 CFR 32, Contract Financing.</t>
+  </si>
+  <si>
+    <t>Determine proper payable amount and other payable information consistent with FASAB Handbook, 48 CFR 32, and Federal Acquisition Regulation (FAR) and as specified in the TFM.</t>
+  </si>
+  <si>
+    <t>TFM Volume I, Part 4A, Chapter 2000 Overall Disbursing Rules for All Federal Agencies, Section 2070 Preaudit of Vouchers;TFM Volume I, Part 4A, Chapter 3000 Requirements for Scheduling Payments Disbursed by the Bureau of the Fiscal Service;SFFAS 1: Accounting for Selected Assets and Liabilities;SFFAS 2: Accounting for Direct Loans and Loan Guarantees;SFFAS 5: Accounting for Liabilities of the Federal Government;SFFAS 12: Recognition of Contingent Liabilities Arising from Litigation: An Amendment of SFFAS 5, Accounting for Liabilities of the Federal Government;SFFAS 17: Accounting for Social Insurance;SFFAS 18: Amendments to Accounting Standards for Direct Loans and Loan Guarantees in SFFAS 2;SFFAS 19: Technical Amendments to Accounting Standards for Direct Loans and Loan Guarantees in SFFAS 2;SFFAS 51: Insurance Programs;48 CFR 32, Contract Financing;FAR 32.905, Payment Documentation and Process</t>
   </si>
 </sst>
 </file>
@@ -787,12 +787,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1109,14 +1109,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="6" width="54" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="5" width="54" customWidth="1"/>
+    <col min="6" max="6" width="101.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1666,12 +1667,12 @@
         <v>102</v>
       </c>
       <c r="F28" t="s">
-        <v>103</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B29" t="s">
         <v>100</v>
@@ -1683,15 +1684,15 @@
         <v>24</v>
       </c>
       <c r="E29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" t="s">
         <v>105</v>
-      </c>
-      <c r="F29" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
         <v>100</v>
@@ -1703,7 +1704,7 @@
         <v>42</v>
       </c>
       <c r="E30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F30" t="s">
         <v>61</v>
@@ -1711,159 +1712,159 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B31" t="s">
         <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D31" t="s">
         <v>24</v>
       </c>
       <c r="E31" t="s">
+        <v>110</v>
+      </c>
+      <c r="F31" t="s">
         <v>111</v>
-      </c>
-      <c r="F31" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
         <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D32" t="s">
         <v>24</v>
       </c>
       <c r="E32" t="s">
+        <v>113</v>
+      </c>
+      <c r="F32" t="s">
         <v>114</v>
-      </c>
-      <c r="F32" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s">
         <v>100</v>
       </c>
       <c r="C33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D33" t="s">
         <v>42</v>
       </c>
       <c r="E33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B34" t="s">
         <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D34" t="s">
-        <v>120</v>
+        <v>42</v>
       </c>
       <c r="E34" t="s">
-        <v>42</v>
+        <v>238</v>
       </c>
       <c r="F34" t="s">
-        <v>121</v>
+        <v>239</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B35" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F35" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D36" t="s">
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F36" t="s">
-        <v>129</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B37" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C37" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D37" t="s">
         <v>24</v>
       </c>
       <c r="E37" t="s">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="F37" t="s">
-        <v>133</v>
+        <v>242</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B38" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C38" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D38" t="s">
         <v>42</v>
       </c>
       <c r="E38" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F38" t="s">
         <v>61</v>
@@ -1871,119 +1872,119 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B39" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D39" t="s">
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F39" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B40" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C40" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D40" t="s">
         <v>24</v>
       </c>
       <c r="E40" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F40" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C41" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D41" t="s">
         <v>42</v>
       </c>
       <c r="E41" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F41" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B42" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D42" t="s">
         <v>42</v>
       </c>
       <c r="E42" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F42" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D43" t="s">
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F43" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B44" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D44" t="s">
         <v>10</v>
       </c>
       <c r="E44" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F44" t="s">
         <v>61</v>
@@ -1991,259 +1992,259 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D45" t="s">
         <v>42</v>
       </c>
       <c r="E45" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F45" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B46" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C46" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D46" t="s">
         <v>42</v>
       </c>
       <c r="E46" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F46" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B47" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C47" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D47" t="s">
         <v>42</v>
       </c>
       <c r="E47" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F47" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B48" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C48" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D48" t="s">
         <v>10</v>
       </c>
       <c r="E48" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F48" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B49" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C49" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D49" t="s">
         <v>24</v>
       </c>
       <c r="E49" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F49" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B50" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C50" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D50" t="s">
         <v>42</v>
       </c>
       <c r="E50" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F50" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B51" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C51" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D51" t="s">
         <v>10</v>
       </c>
       <c r="E51" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F51" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B52" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C52" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D52" t="s">
         <v>24</v>
       </c>
       <c r="E52" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F52" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B53" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C53" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D53" t="s">
         <v>24</v>
       </c>
       <c r="E53" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F53" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C54" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D54" t="s">
         <v>24</v>
       </c>
       <c r="E54" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F54" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B55" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C55" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D55" t="s">
         <v>10</v>
       </c>
       <c r="E55" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F55" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B56" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C56" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D56" t="s">
         <v>24</v>
       </c>
       <c r="E56" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F56" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B57" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C57" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="D57" t="s">
         <v>42</v>
       </c>
       <c r="E57" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F57" t="s">
         <v>61</v>
@@ -2251,119 +2252,119 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B58" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C58" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D58" t="s">
         <v>42</v>
       </c>
       <c r="E58" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F58" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B59" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D59" t="s">
         <v>42</v>
       </c>
       <c r="E59" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="F59" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B60" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C60" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D60" t="s">
         <v>10</v>
       </c>
       <c r="E60" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F60" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B61" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C61" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D61" t="s">
         <v>24</v>
       </c>
       <c r="E61" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F61" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B62" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C62" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D62" t="s">
         <v>42</v>
       </c>
       <c r="E62" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F62" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B63" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C63" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D63" t="s">
         <v>42</v>
       </c>
       <c r="E63" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="F63" t="s">
         <v>61</v>
@@ -2371,7 +2372,7 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B64" t="s">
         <v>78</v>
@@ -2383,15 +2384,15 @@
         <v>24</v>
       </c>
       <c r="E64" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F64" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B65" t="s">
         <v>78</v>
@@ -2403,55 +2404,55 @@
         <v>24</v>
       </c>
       <c r="E65" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F65" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B66" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C66" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D66" t="s">
         <v>24</v>
       </c>
       <c r="E66" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F66" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B67" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C67" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D67" t="s">
         <v>24</v>
       </c>
       <c r="E67" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="F67" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B68" t="s">
         <v>34</v>
@@ -2460,10 +2461,10 @@
         <v>35</v>
       </c>
       <c r="D68" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E68" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="F68" t="s">
         <v>61</v>
@@ -2471,7 +2472,7 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B69" t="s">
         <v>34</v>
@@ -2483,15 +2484,15 @@
         <v>10</v>
       </c>
       <c r="E69" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="F69" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B70" t="s">
         <v>8</v>
@@ -2503,10 +2504,10 @@
         <v>24</v>
       </c>
       <c r="E70" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="F70" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>